<commit_message>
add RAF Lyneham data
</commit_message>
<xml_diff>
--- a/Building Characteristics.xlsx
+++ b/Building Characteristics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\ZHAW\EVA_DMBEM\Group Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\Documents\GitHub\DMBEM-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B1869A-8875-43A1-B9CE-857EC72C6FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73636394-4470-4587-A43A-EE661D2ABB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AD515140-1401-474E-BFE0-96FA6661CFBA}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
-    <t>Element Code</t>
-  </si>
-  <si>
     <t>W1</t>
   </si>
   <si>
@@ -72,39 +69,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Length (m)</t>
-  </si>
-  <si>
-    <t>Height (m)</t>
-  </si>
-  <si>
-    <t>Surface (m2)</t>
-  </si>
-  <si>
-    <t>Width (m)</t>
-  </si>
-  <si>
-    <t>Element Type</t>
-  </si>
-  <si>
-    <t>Material 1</t>
-  </si>
-  <si>
-    <t>Material 2</t>
-  </si>
-  <si>
-    <t>Material 3</t>
-  </si>
-  <si>
-    <t>Thickness 1 (m)</t>
-  </si>
-  <si>
-    <t>Thickness 2 (m)</t>
-  </si>
-  <si>
-    <t>Thickness 3 (m)</t>
-  </si>
-  <si>
     <t>Wood</t>
   </si>
   <si>
@@ -114,9 +78,6 @@
     <t>Slope</t>
   </si>
   <si>
-    <t>Volume (m3)</t>
-  </si>
-  <si>
     <t>SinG</t>
   </si>
   <si>
@@ -130,6 +91,45 @@
   </si>
   <si>
     <t>Azimuth</t>
+  </si>
+  <si>
+    <t>Element_Type</t>
+  </si>
+  <si>
+    <t>Element_Code</t>
+  </si>
+  <si>
+    <t>Material_1</t>
+  </si>
+  <si>
+    <t>Material_2</t>
+  </si>
+  <si>
+    <t>Material_3</t>
+  </si>
+  <si>
+    <t>Length_m</t>
+  </si>
+  <si>
+    <t>Width_m</t>
+  </si>
+  <si>
+    <t>Height_m</t>
+  </si>
+  <si>
+    <t>Thickness_1_m</t>
+  </si>
+  <si>
+    <t>Thickness_2_m</t>
+  </si>
+  <si>
+    <t>Thickness_3_m</t>
+  </si>
+  <si>
+    <t>Surface_m2</t>
+  </si>
+  <si>
+    <t>Volume_m3</t>
   </si>
 </sst>
 </file>
@@ -485,16 +485,15 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
@@ -505,69 +504,69 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -582,14 +581,14 @@
         <v>0.1</v>
       </c>
       <c r="K2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L2">
         <f>G2*H2</f>
         <v>6</v>
       </c>
       <c r="M2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N2">
         <v>90</v>
@@ -600,25 +599,25 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3">
         <v>3</v>
@@ -630,14 +629,14 @@
         <v>0.1</v>
       </c>
       <c r="K3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L3">
         <f>F3*H3</f>
         <v>9</v>
       </c>
       <c r="M3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N3">
         <v>90</v>
@@ -648,22 +647,22 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -678,14 +677,14 @@
         <v>0.1</v>
       </c>
       <c r="K4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L4">
         <f>H4*G4</f>
         <v>6</v>
       </c>
       <c r="M4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N4">
         <v>90</v>
@@ -696,25 +695,25 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5">
         <v>3</v>
@@ -723,17 +722,17 @@
         <v>0.1</v>
       </c>
       <c r="J5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L5">
         <f>H5*F5</f>
         <v>9</v>
       </c>
       <c r="M5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N5">
         <v>90</v>
@@ -744,19 +743,19 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -774,7 +773,7 @@
         <v>0.4</v>
       </c>
       <c r="K6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L6">
         <f>F6*G6</f>
@@ -793,19 +792,19 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -823,14 +822,14 @@
         <v>0.3</v>
       </c>
       <c r="K7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L7">
         <f>F7*G7</f>
         <v>6</v>
       </c>
       <c r="M7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N7">
         <v>0</v>

</xml_diff>

<commit_message>
smaller window, fourth wall
</commit_message>
<xml_diff>
--- a/Building Characteristics.xlsx
+++ b/Building Characteristics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\GitHub\DMBEM-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leni\Nextcloud\Lena\ZHAW\HS 21\EVA_DMBEM\DMBEM-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B42C10-993E-4C13-ABAE-FA7974C3FF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A01F407-E572-496E-B1D7-39682EBAF8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AD515140-1401-474E-BFE0-96FA6661CFBA}"/>
+    <workbookView xWindow="11496" yWindow="24" windowWidth="11544" windowHeight="12480" xr2:uid="{AD515140-1401-474E-BFE0-96FA6661CFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>W1</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>R2</t>
+  </si>
+  <si>
+    <t>W4</t>
   </si>
 </sst>
 </file>
@@ -189,7 +192,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -485,13 +488,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22378C7-BEBB-44C6-ACEE-376CBFA0A07A}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
@@ -590,7 +593,7 @@
         <v>6</v>
       </c>
       <c r="M2">
-        <f>F8*G8*H8</f>
+        <f>F9*G9*H9</f>
         <v>18</v>
       </c>
       <c r="N2">
@@ -692,16 +695,16 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -718,15 +721,15 @@
       <c r="I5">
         <v>0.1</v>
       </c>
-      <c r="J5" t="s">
-        <v>10</v>
+      <c r="J5">
+        <v>0.1</v>
       </c>
       <c r="K5" t="s">
         <v>10</v>
       </c>
       <c r="L5">
-        <f>H5*F5</f>
-        <v>9</v>
+        <f>F5*H5 - L6</f>
+        <v>2.75</v>
       </c>
       <c r="N5">
         <v>90</v>
@@ -737,52 +740,52 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
+        <v>2.5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="I6">
-        <v>0.3</v>
-      </c>
-      <c r="J6">
-        <v>0.3</v>
+        <v>0.1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
       </c>
       <c r="K6" t="s">
         <v>10</v>
       </c>
       <c r="L6">
-        <f>F6*G6</f>
-        <v>6</v>
+        <f>H6*F6</f>
+        <v>6.25</v>
       </c>
       <c r="N6">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="O6">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -822,21 +825,21 @@
         <v>45</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -851,10 +854,10 @@
         <v>3</v>
       </c>
       <c r="I8">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="J8">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="K8" t="s">
         <v>10</v>
@@ -864,9 +867,54 @@
         <v>6</v>
       </c>
       <c r="N8">
+        <v>45</v>
+      </c>
+      <c r="O8">
         <v>0</v>
       </c>
-      <c r="O8">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>0.1</v>
+      </c>
+      <c r="J9">
+        <v>0.4</v>
+      </c>
+      <c r="K9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9">
+        <f>F9*G9</f>
+        <v>6</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
         <v>0</v>
       </c>
     </row>

</xml_diff>